<commit_message>
update the result generating script
</commit_message>
<xml_diff>
--- a/result/result_Total_back5.xlsx
+++ b/result/result_Total_back5.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:F166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,34 +439,51 @@
           <t>NOC</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>SVM</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>RandomForest</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>DicisionTree</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>DecisionTree</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>LinearRegression</t>
         </is>
       </c>
-    </row>
-    <row r="2"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
           <t>Afghanistan</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -474,6 +491,21 @@
           <t>Albania</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>2.933575947555603</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.8805391171783699</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -481,6 +513,21 @@
           <t>Algeria</t>
         </is>
       </c>
+      <c r="B5" t="n">
+        <v>2.795963766787715</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5.628856671724344</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -489,16 +536,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>7.687032884447568</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>6.72</v>
       </c>
       <c r="D6" t="n">
         <v>8</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4.519438406769719</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -508,15 +558,18 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>4.494072225247088</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>3.14</v>
       </c>
       <c r="D7" t="n">
         <v>4</v>
       </c>
       <c r="E7" t="n">
+        <v>2.899167533244515</v>
+      </c>
+      <c r="F7" t="n">
         <v>3</v>
       </c>
     </row>
@@ -526,6 +579,31 @@
           <t>Australasia</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -534,16 +612,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49</v>
+        <v>49.40857565542284</v>
       </c>
       <c r="C9" t="n">
-        <v>47</v>
+        <v>47.06</v>
       </c>
       <c r="D9" t="n">
         <v>33</v>
       </c>
       <c r="E9" t="n">
-        <v>55</v>
+        <v>54.99348447256061</v>
+      </c>
+      <c r="F9" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="10">
@@ -553,15 +634,18 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>6.831860306023529</v>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>5.84</v>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>5.423076923076923</v>
       </c>
       <c r="E10" t="n">
+        <v>5.275533779854358</v>
+      </c>
+      <c r="F10" t="n">
         <v>5</v>
       </c>
     </row>
@@ -572,15 +656,18 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>6.886657020433127</v>
       </c>
       <c r="C11" t="n">
-        <v>9</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="D11" t="n">
-        <v>7</v>
+        <v>6.714285714285714</v>
       </c>
       <c r="E11" t="n">
+        <v>6.552406478768109</v>
+      </c>
+      <c r="F11" t="n">
         <v>7</v>
       </c>
     </row>
@@ -590,6 +677,21 @@
           <t>Bahamas</t>
         </is>
       </c>
+      <c r="B12" t="n">
+        <v>2.075713252653969</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.358024691358025</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.365506212637169</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -598,16 +700,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>4.351747380834311</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>3.35</v>
       </c>
       <c r="D13" t="n">
         <v>4</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>2.399033068677074</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -616,6 +721,11 @@
           <t>Barbados</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -623,6 +733,21 @@
           <t>Belarus</t>
         </is>
       </c>
+      <c r="B15" t="n">
+        <v>15.50957666130017</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13.21868037072485</v>
+      </c>
+      <c r="F15" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -631,16 +756,19 @@
         </is>
       </c>
       <c r="B16" t="n">
+        <v>7.989202671239632</v>
+      </c>
+      <c r="C16" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6.45</v>
+      </c>
+      <c r="E16" t="n">
+        <v>9.001532963552203</v>
+      </c>
+      <c r="F16" t="n">
         <v>8</v>
-      </c>
-      <c r="C16" t="n">
-        <v>9</v>
-      </c>
-      <c r="D16" t="n">
-        <v>6</v>
-      </c>
-      <c r="E16" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="17">
@@ -649,6 +777,21 @@
           <t>Bermuda</t>
         </is>
       </c>
+      <c r="B17" t="n">
+        <v>2.477295224051709</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.672047619047619</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.918734378380532</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -656,6 +799,31 @@
           <t>Bohemia</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -663,6 +831,21 @@
           <t>Botswana</t>
         </is>
       </c>
+      <c r="B19" t="n">
+        <v>2.912471633565929</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2.282505489135738</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -671,16 +854,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>24</v>
+        <v>24.17083318915026</v>
       </c>
       <c r="C20" t="n">
-        <v>25</v>
+        <v>24.73</v>
       </c>
       <c r="D20" t="n">
-        <v>19</v>
+        <v>18.90909090909091</v>
       </c>
       <c r="E20" t="n">
-        <v>23</v>
+        <v>22.69420645855344</v>
+      </c>
+      <c r="F20" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -689,6 +875,31 @@
           <t>British West Indies</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -697,15 +908,18 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>8</v>
+        <v>7.742795979792376</v>
       </c>
       <c r="C22" t="n">
-        <v>8</v>
+        <v>7.86</v>
       </c>
       <c r="D22" t="n">
-        <v>6</v>
+        <v>6.45</v>
       </c>
       <c r="E22" t="n">
+        <v>7.266304066259252</v>
+      </c>
+      <c r="F22" t="n">
         <v>7</v>
       </c>
     </row>
@@ -715,6 +929,21 @@
           <t>Burkina Faso</t>
         </is>
       </c>
+      <c r="B23" t="n">
+        <v>2.484955997609156</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.662047619047619</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.8770639178866038</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -722,6 +951,21 @@
           <t>Burundi</t>
         </is>
       </c>
+      <c r="B24" t="n">
+        <v>2.5857505784493</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.768809523809524</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2135125859334757</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -729,6 +973,21 @@
           <t>Cabo Verde</t>
         </is>
       </c>
+      <c r="B25" t="n">
+        <v>2.746809442882174</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1.486666666666667</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.5339402483758207</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -736,6 +995,11 @@
           <t>Cameroon</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -744,16 +1008,19 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>32</v>
+        <v>32.4166978164743</v>
       </c>
       <c r="C27" t="n">
-        <v>35</v>
+        <v>34.76</v>
       </c>
       <c r="D27" t="n">
         <v>34</v>
       </c>
       <c r="E27" t="n">
-        <v>30</v>
+        <v>30.38000719551395</v>
+      </c>
+      <c r="F27" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="28">
@@ -762,6 +1029,11 @@
           <t>Ceylon</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -769,6 +1041,21 @@
           <t>Chile</t>
         </is>
       </c>
+      <c r="B29" t="n">
+        <v>2.476766757436557</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.358024691358025</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.444892583657711</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -777,16 +1064,19 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>98</v>
+        <v>98.03702382310368</v>
       </c>
       <c r="C30" t="n">
-        <v>100</v>
+        <v>100.11</v>
       </c>
       <c r="D30" t="n">
         <v>121</v>
       </c>
       <c r="E30" t="n">
-        <v>92</v>
+        <v>92.16359263401519</v>
+      </c>
+      <c r="F30" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="31">
@@ -796,15 +1086,18 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>8</v>
+        <v>7.7497853415124</v>
       </c>
       <c r="C31" t="n">
-        <v>7</v>
+        <v>6.99</v>
       </c>
       <c r="D31" t="n">
-        <v>6</v>
+        <v>6.45</v>
       </c>
       <c r="E31" t="n">
+        <v>7.142420197603663</v>
+      </c>
+      <c r="F31" t="n">
         <v>7</v>
       </c>
     </row>
@@ -815,15 +1108,18 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5</v>
+        <v>4.790045930484183</v>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>4.62</v>
       </c>
       <c r="D32" t="n">
-        <v>4</v>
+        <v>3.909090909090909</v>
       </c>
       <c r="E32" t="n">
+        <v>4.373714659823355</v>
+      </c>
+      <c r="F32" t="n">
         <v>4</v>
       </c>
     </row>
@@ -833,6 +1129,11 @@
           <t>Costa Rica</t>
         </is>
       </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -841,15 +1142,18 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>7</v>
+        <v>6.546008136006584</v>
       </c>
       <c r="C34" t="n">
-        <v>8</v>
+        <v>7.93</v>
       </c>
       <c r="D34" t="n">
-        <v>10</v>
+        <v>9.76923076923077</v>
       </c>
       <c r="E34" t="n">
+        <v>6.861530807873731</v>
+      </c>
+      <c r="F34" t="n">
         <v>7</v>
       </c>
     </row>
@@ -860,16 +1164,19 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>16</v>
+        <v>15.82246566319691</v>
       </c>
       <c r="C35" t="n">
-        <v>11</v>
+        <v>10.76</v>
       </c>
       <c r="D35" t="n">
         <v>13</v>
       </c>
       <c r="E35" t="n">
-        <v>11</v>
+        <v>11.41986578663366</v>
+      </c>
+      <c r="F35" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="36">
@@ -878,6 +1185,21 @@
           <t>Cyprus</t>
         </is>
       </c>
+      <c r="B36" t="n">
+        <v>2.752897344907268</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.413741804644927</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -886,16 +1208,19 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>7</v>
+        <v>6.696512935207863</v>
       </c>
       <c r="C37" t="n">
-        <v>7</v>
+        <v>6.65</v>
       </c>
       <c r="D37" t="n">
         <v>8</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6.523002673008131</v>
+      </c>
+      <c r="F37" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="38">
@@ -924,6 +1249,11 @@
           <t>ABSENT</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -932,16 +1262,19 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>9</v>
+        <v>8.500953136602263</v>
       </c>
       <c r="C39" t="n">
-        <v>9</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="D39" t="n">
-        <v>7</v>
+        <v>6.714285714285714</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>9.396820511571194</v>
+      </c>
+      <c r="F39" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -950,6 +1283,11 @@
           <t>Djibouti</t>
         </is>
       </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -957,6 +1295,21 @@
           <t>Dominica</t>
         </is>
       </c>
+      <c r="B41" t="n">
+        <v>2.837961892642326</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1.566666666666667</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.1283529360802884</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -965,15 +1318,18 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>4.393614094047066</v>
       </c>
       <c r="C42" t="n">
-        <v>3</v>
+        <v>3.37</v>
       </c>
       <c r="D42" t="n">
-        <v>4</v>
+        <v>3.909090909090909</v>
       </c>
       <c r="E42" t="n">
+        <v>2.623927256413449</v>
+      </c>
+      <c r="F42" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1003,6 +1359,11 @@
           <t>ABSENT</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1010,6 +1371,21 @@
           <t>Ecuador</t>
         </is>
       </c>
+      <c r="B44" t="n">
+        <v>3.267203951319068</v>
+      </c>
+      <c r="C44" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" t="n">
+        <v>4.641090581683232</v>
+      </c>
+      <c r="F44" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1018,16 +1394,19 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>6</v>
+        <v>5.716822094893203</v>
       </c>
       <c r="C45" t="n">
-        <v>6</v>
+        <v>5.89</v>
       </c>
       <c r="D45" t="n">
+        <v>5.423076923076923</v>
+      </c>
+      <c r="E45" t="n">
+        <v>4.034306443289418</v>
+      </c>
+      <c r="F45" t="n">
         <v>5</v>
-      </c>
-      <c r="E45" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="46">
@@ -1036,6 +1415,11 @@
           <t>Eritrea</t>
         </is>
       </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1043,6 +1427,21 @@
           <t>Estonia</t>
         </is>
       </c>
+      <c r="B47" t="n">
+        <v>2.399941514265279</v>
+      </c>
+      <c r="C47" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="D47" t="n">
+        <v>2.285714285714286</v>
+      </c>
+      <c r="E47" t="n">
+        <v>5.134175511341277</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1051,15 +1450,18 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>4</v>
+        <v>4.096207079898747</v>
       </c>
       <c r="C48" t="n">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="D48" t="n">
-        <v>3</v>
+        <v>3.375</v>
       </c>
       <c r="E48" t="n">
+        <v>3.362294559941061</v>
+      </c>
+      <c r="F48" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1069,6 +1471,31 @@
           <t>FR Yugoslavia</t>
         </is>
       </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1076,6 +1503,21 @@
           <t>Fiji</t>
         </is>
       </c>
+      <c r="B50" t="n">
+        <v>2.281569250205294</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1.358024691358025</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3.154473755030968</v>
+      </c>
+      <c r="F50" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1083,6 +1525,21 @@
           <t>Finland</t>
         </is>
       </c>
+      <c r="B51" t="n">
+        <v>3.414784331204871</v>
+      </c>
+      <c r="C51" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="D51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E51" t="n">
+        <v>8.288434420622947</v>
+      </c>
+      <c r="F51" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1090,6 +1547,11 @@
           <t>Formosa</t>
         </is>
       </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1098,16 +1560,19 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>49</v>
+        <v>49.28130904939668</v>
       </c>
       <c r="C53" t="n">
-        <v>60</v>
+        <v>60.17</v>
       </c>
       <c r="D53" t="n">
         <v>45</v>
       </c>
       <c r="E53" t="n">
-        <v>59</v>
+        <v>59.48854027822784</v>
+      </c>
+      <c r="F53" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="54">
@@ -1116,6 +1581,11 @@
           <t>Gabon</t>
         </is>
       </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1124,16 +1594,19 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>6</v>
+        <v>5.753433408254381</v>
       </c>
       <c r="C55" t="n">
+        <v>7.29</v>
+      </c>
+      <c r="D55" t="n">
+        <v>9.76923076923077</v>
+      </c>
+      <c r="E55" t="n">
+        <v>6.062771435093019</v>
+      </c>
+      <c r="F55" t="n">
         <v>7</v>
-      </c>
-      <c r="D55" t="n">
-        <v>10</v>
-      </c>
-      <c r="E55" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="56">
@@ -1143,16 +1616,19 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>43</v>
+        <v>42.64276292362899</v>
       </c>
       <c r="C56" t="n">
-        <v>50</v>
+        <v>49.88</v>
       </c>
       <c r="D56" t="n">
         <v>64</v>
       </c>
       <c r="E56" t="n">
-        <v>40</v>
+        <v>39.69178969021799</v>
+      </c>
+      <c r="F56" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="57">
@@ -1161,6 +1637,21 @@
           <t>Ghana</t>
         </is>
       </c>
+      <c r="B57" t="n">
+        <v>2.371489198899191</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1.766666666666667</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1.629579227644521</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1169,16 +1660,19 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>58</v>
+        <v>57.7688322984398</v>
       </c>
       <c r="C58" t="n">
-        <v>65</v>
+        <v>65.48</v>
       </c>
       <c r="D58" t="n">
-        <v>65</v>
+        <v>64.66666666666667</v>
       </c>
       <c r="E58" t="n">
-        <v>66</v>
+        <v>66.06106957548506</v>
+      </c>
+      <c r="F58" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="59">
@@ -1188,15 +1682,18 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>7</v>
+        <v>7.331515501818458</v>
       </c>
       <c r="C59" t="n">
-        <v>7</v>
+        <v>7.4</v>
       </c>
       <c r="D59" t="n">
-        <v>6</v>
+        <v>6.45</v>
       </c>
       <c r="E59" t="n">
+        <v>7.333575276620573</v>
+      </c>
+      <c r="F59" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1206,6 +1703,21 @@
           <t>Grenada</t>
         </is>
       </c>
+      <c r="B60" t="n">
+        <v>3.036790132829182</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1.683333333333333</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1.274644122167353</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1213,6 +1725,21 @@
           <t>Guatemala</t>
         </is>
       </c>
+      <c r="B61" t="n">
+        <v>2.951119460940504</v>
+      </c>
+      <c r="C61" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2.640985914174231</v>
+      </c>
+      <c r="F61" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1220,6 +1747,11 @@
           <t>Guyana</t>
         </is>
       </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1227,6 +1759,11 @@
           <t>Haiti</t>
         </is>
       </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1234,6 +1771,21 @@
           <t>Hong Kong</t>
         </is>
       </c>
+      <c r="B64" t="n">
+        <v>3.701281388785574</v>
+      </c>
+      <c r="C64" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="D64" t="n">
+        <v>5</v>
+      </c>
+      <c r="E64" t="n">
+        <v>8.590097948891195</v>
+      </c>
+      <c r="F64" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1242,16 +1794,19 @@
         </is>
       </c>
       <c r="B65" t="n">
+        <v>19.34068256437053</v>
+      </c>
+      <c r="C65" t="n">
+        <v>17.79</v>
+      </c>
+      <c r="D65" t="n">
+        <v>18.90909090909091</v>
+      </c>
+      <c r="E65" t="n">
+        <v>20.88971867381324</v>
+      </c>
+      <c r="F65" t="n">
         <v>19</v>
-      </c>
-      <c r="C65" t="n">
-        <v>18</v>
-      </c>
-      <c r="D65" t="n">
-        <v>19</v>
-      </c>
-      <c r="E65" t="n">
-        <v>21</v>
       </c>
     </row>
     <row r="66">
@@ -1260,6 +1815,11 @@
           <t>Iceland</t>
         </is>
       </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1267,6 +1827,31 @@
           <t>Independent Olympic Athletes</t>
         </is>
       </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1274,6 +1859,31 @@
           <t>Independent Olympic Participants</t>
         </is>
       </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1282,16 +1892,19 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>6</v>
+        <v>5.872521108975093</v>
       </c>
       <c r="C69" t="n">
-        <v>6</v>
+        <v>5.63</v>
       </c>
       <c r="D69" t="n">
+        <v>5.423076923076923</v>
+      </c>
+      <c r="E69" t="n">
+        <v>6.005005484828668</v>
+      </c>
+      <c r="F69" t="n">
         <v>5</v>
-      </c>
-      <c r="E69" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="70">
@@ -1301,15 +1914,18 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>4</v>
+        <v>4.306482786573071</v>
       </c>
       <c r="C70" t="n">
-        <v>2</v>
+        <v>2.15</v>
       </c>
       <c r="D70" t="n">
-        <v>3</v>
+        <v>3.375</v>
       </c>
       <c r="E70" t="n">
+        <v>2.637855696686065</v>
+      </c>
+      <c r="F70" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1320,16 +1936,19 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>7</v>
+        <v>7.372604572316448</v>
       </c>
       <c r="C71" t="n">
-        <v>9</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="D71" t="n">
         <v>7</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>10.01384598301015</v>
+      </c>
+      <c r="F71" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="72">
@@ -1338,6 +1957,11 @@
           <t>Iraq</t>
         </is>
       </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1346,15 +1970,18 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>6</v>
+        <v>5.815513631846052</v>
       </c>
       <c r="C73" t="n">
-        <v>6</v>
+        <v>6.32</v>
       </c>
       <c r="D73" t="n">
-        <v>6</v>
+        <v>6.45</v>
       </c>
       <c r="E73" t="n">
+        <v>6.365713422812714</v>
+      </c>
+      <c r="F73" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1365,15 +1992,18 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>6</v>
+        <v>6.45902848367038</v>
       </c>
       <c r="C74" t="n">
-        <v>7</v>
+        <v>6.62</v>
       </c>
       <c r="D74" t="n">
-        <v>6</v>
+        <v>6.45</v>
       </c>
       <c r="E74" t="n">
+        <v>5.93703450925039</v>
+      </c>
+      <c r="F74" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1384,16 +2014,19 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>42</v>
+        <v>42.25915387078318</v>
       </c>
       <c r="C75" t="n">
-        <v>38</v>
+        <v>38.32</v>
       </c>
       <c r="D75" t="n">
         <v>40</v>
       </c>
       <c r="E75" t="n">
-        <v>42</v>
+        <v>42.43898249033999</v>
+      </c>
+      <c r="F75" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="76">
@@ -1402,6 +2035,21 @@
           <t>Ivory Coast</t>
         </is>
       </c>
+      <c r="B76" t="n">
+        <v>2.502810156830137</v>
+      </c>
+      <c r="C76" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1.397865372129608</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1410,15 +2058,18 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>6</v>
+        <v>5.759856115309091</v>
       </c>
       <c r="C77" t="n">
-        <v>7</v>
+        <v>6.59</v>
       </c>
       <c r="D77" t="n">
-        <v>6</v>
+        <v>6.444444444444445</v>
       </c>
       <c r="E77" t="n">
+        <v>6.445680160251641</v>
+      </c>
+      <c r="F77" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1429,16 +2080,19 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>46</v>
+        <v>45.61074729752478</v>
       </c>
       <c r="C78" t="n">
-        <v>42</v>
+        <v>41.53</v>
       </c>
       <c r="D78" t="n">
         <v>40</v>
       </c>
       <c r="E78" t="n">
-        <v>50</v>
+        <v>49.65204259999228</v>
+      </c>
+      <c r="F78" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="79">
@@ -1447,6 +2101,21 @@
           <t>Jordan</t>
         </is>
       </c>
+      <c r="B79" t="n">
+        <v>2.500068404106557</v>
+      </c>
+      <c r="C79" t="n">
+        <v>1.773333333333333</v>
+      </c>
+      <c r="D79" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E79" t="n">
+        <v>1.356945068299635</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1455,15 +2124,18 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>7</v>
+        <v>7.248940853439521</v>
       </c>
       <c r="C80" t="n">
-        <v>8</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="D80" t="n">
-        <v>7</v>
+        <v>6.714285714285714</v>
       </c>
       <c r="E80" t="n">
+        <v>7.394396654268721</v>
+      </c>
+      <c r="F80" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1474,16 +2146,19 @@
         </is>
       </c>
       <c r="B81" t="n">
+        <v>7.837931612781539</v>
+      </c>
+      <c r="C81" t="n">
+        <v>8.81</v>
+      </c>
+      <c r="D81" t="n">
+        <v>6.714285714285714</v>
+      </c>
+      <c r="E81" t="n">
+        <v>10.27832472568231</v>
+      </c>
+      <c r="F81" t="n">
         <v>8</v>
-      </c>
-      <c r="C81" t="n">
-        <v>9</v>
-      </c>
-      <c r="D81" t="n">
-        <v>7</v>
-      </c>
-      <c r="E81" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="82">
@@ -1492,6 +2167,21 @@
           <t>Kosovo</t>
         </is>
       </c>
+      <c r="B82" t="n">
+        <v>2.727803240895369</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1.893333333333334</v>
+      </c>
+      <c r="D82" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E82" t="n">
+        <v>1.396938525533393</v>
+      </c>
+      <c r="F82" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1499,6 +2189,21 @@
           <t>Kuwait</t>
         </is>
       </c>
+      <c r="B83" t="n">
+        <v>2.589962448348984</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1.458714285714286</v>
+      </c>
+      <c r="D83" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1.898828629871365</v>
+      </c>
+      <c r="F83" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1506,6 +2211,21 @@
           <t>Kyrgyzstan</t>
         </is>
       </c>
+      <c r="B84" t="n">
+        <v>4.547203286216501</v>
+      </c>
+      <c r="C84" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="D84" t="n">
+        <v>2</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1.694974766731791</v>
+      </c>
+      <c r="F84" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1513,6 +2233,21 @@
           <t>Latvia</t>
         </is>
       </c>
+      <c r="B85" t="n">
+        <v>2.496578149809366</v>
+      </c>
+      <c r="C85" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="D85" t="n">
+        <v>2.285714285714286</v>
+      </c>
+      <c r="E85" t="n">
+        <v>5.507025666389703</v>
+      </c>
+      <c r="F85" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1520,6 +2255,11 @@
           <t>Lebanon</t>
         </is>
       </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1528,16 +2268,19 @@
         </is>
       </c>
       <c r="B87" t="n">
+        <v>4.479598494047778</v>
+      </c>
+      <c r="C87" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="D87" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="E87" t="n">
+        <v>3.407556708149283</v>
+      </c>
+      <c r="F87" t="n">
         <v>4</v>
-      </c>
-      <c r="C87" t="n">
-        <v>5</v>
-      </c>
-      <c r="D87" t="n">
-        <v>4</v>
-      </c>
-      <c r="E87" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -1546,6 +2289,11 @@
           <t>Luxembourg</t>
         </is>
       </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1553,6 +2301,11 @@
           <t>Macedonia</t>
         </is>
       </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1561,16 +2314,19 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>4</v>
+        <v>3.833635631771934</v>
       </c>
       <c r="C90" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="D90" t="n">
-        <v>3</v>
+        <v>3.375</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>1.289412750090403</v>
+      </c>
+      <c r="F90" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -1579,6 +2335,11 @@
           <t>Mauritius</t>
         </is>
       </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="inlineStr"/>
+      <c r="F91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1587,16 +2348,19 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>7</v>
+        <v>6.524634663055387</v>
       </c>
       <c r="C92" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="D92" t="n">
+        <v>4.176470588235294</v>
+      </c>
+      <c r="E92" t="n">
+        <v>5.879676876883233</v>
+      </c>
+      <c r="F92" t="n">
         <v>5</v>
-      </c>
-      <c r="D92" t="n">
-        <v>4</v>
-      </c>
-      <c r="E92" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="93">
@@ -1625,6 +2389,11 @@
           <t>ABSENT</t>
         </is>
       </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1632,6 +2401,21 @@
           <t>Moldova</t>
         </is>
       </c>
+      <c r="B94" t="n">
+        <v>3.174344435947845</v>
+      </c>
+      <c r="C94" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="D94" t="n">
+        <v>2</v>
+      </c>
+      <c r="E94" t="n">
+        <v>2.189176100326834</v>
+      </c>
+      <c r="F94" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1640,16 +2424,19 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>3</v>
+        <v>3.280906988401249</v>
       </c>
       <c r="C95" t="n">
-        <v>3</v>
+        <v>2.84</v>
       </c>
       <c r="D95" t="n">
-        <v>3</v>
+        <v>3.375</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>0.969345267686224</v>
+      </c>
+      <c r="F95" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="96">
@@ -1658,6 +2445,11 @@
           <t>Montenegro</t>
         </is>
       </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1665,6 +2457,21 @@
           <t>Morocco</t>
         </is>
       </c>
+      <c r="B97" t="n">
+        <v>2.34275807786095</v>
+      </c>
+      <c r="C97" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="D97" t="n">
+        <v>4</v>
+      </c>
+      <c r="E97" t="n">
+        <v>5.073894845828443</v>
+      </c>
+      <c r="F97" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1672,6 +2479,11 @@
           <t>Mozambique</t>
         </is>
       </c>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1679,6 +2491,21 @@
           <t>Namibia</t>
         </is>
       </c>
+      <c r="B99" t="n">
+        <v>2.484788097039456</v>
+      </c>
+      <c r="C99" t="n">
+        <v>1.662047619047619</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.8779679684308874</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1687,16 +2514,19 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>34</v>
+        <v>33.78295491806603</v>
       </c>
       <c r="C100" t="n">
-        <v>24</v>
+        <v>23.7</v>
       </c>
       <c r="D100" t="n">
-        <v>22</v>
+        <v>22.23333333333333</v>
       </c>
       <c r="E100" t="n">
-        <v>34</v>
+        <v>34.01393393180953</v>
+      </c>
+      <c r="F100" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="101">
@@ -1705,6 +2535,31 @@
           <t>Netherlands Antilles</t>
         </is>
       </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1713,16 +2568,19 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>17</v>
+        <v>17.40729897317382</v>
       </c>
       <c r="C102" t="n">
-        <v>18</v>
+        <v>17.89</v>
       </c>
       <c r="D102" t="n">
         <v>14</v>
       </c>
       <c r="E102" t="n">
-        <v>20</v>
+        <v>20.24081840425642</v>
+      </c>
+      <c r="F102" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="103">
@@ -1731,6 +2589,21 @@
           <t>Niger</t>
         </is>
       </c>
+      <c r="B103" t="n">
+        <v>2.605484034892903</v>
+      </c>
+      <c r="C103" t="n">
+        <v>1.486666666666667</v>
+      </c>
+      <c r="D103" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.1118607873786033</v>
+      </c>
+      <c r="F103" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1738,6 +2611,21 @@
           <t>Nigeria</t>
         </is>
       </c>
+      <c r="B104" t="n">
+        <v>3.177651528763064</v>
+      </c>
+      <c r="C104" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" t="n">
+        <v>8.419325351685039</v>
+      </c>
+      <c r="F104" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1745,6 +2633,21 @@
           <t>North Korea</t>
         </is>
       </c>
+      <c r="B105" t="n">
+        <v>8.536546382595482</v>
+      </c>
+      <c r="C105" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="D105" t="n">
+        <v>6</v>
+      </c>
+      <c r="E105" t="n">
+        <v>4.238745052221486</v>
+      </c>
+      <c r="F105" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -1752,6 +2655,21 @@
           <t>North Macedonia</t>
         </is>
       </c>
+      <c r="B106" t="n">
+        <v>2.567986025886206</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1.376666666666666</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.4708049478513763</v>
+      </c>
+      <c r="F106" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1760,16 +2678,19 @@
         </is>
       </c>
       <c r="B107" t="n">
+        <v>7.258927519410953</v>
+      </c>
+      <c r="C107" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="D107" t="n">
+        <v>6.45</v>
+      </c>
+      <c r="E107" t="n">
+        <v>7.565422223102351</v>
+      </c>
+      <c r="F107" t="n">
         <v>7</v>
-      </c>
-      <c r="C107" t="n">
-        <v>8</v>
-      </c>
-      <c r="D107" t="n">
-        <v>6</v>
-      </c>
-      <c r="E107" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="108">
@@ -1778,6 +2699,21 @@
           <t>Pakistan</t>
         </is>
       </c>
+      <c r="B108" t="n">
+        <v>2.746936847960001</v>
+      </c>
+      <c r="C108" t="n">
+        <v>1.486666666666667</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.5333234317986539</v>
+      </c>
+      <c r="F108" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -1785,6 +2721,21 @@
           <t>Panama</t>
         </is>
       </c>
+      <c r="B109" t="n">
+        <v>2.503346464016097</v>
+      </c>
+      <c r="C109" t="n">
+        <v>1.856666666666667</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.8756838021944056</v>
+      </c>
+      <c r="F109" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -1792,6 +2743,11 @@
           <t>Paraguay</t>
         </is>
       </c>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -1799,6 +2755,21 @@
           <t>Peru</t>
         </is>
       </c>
+      <c r="B111" t="n">
+        <v>2.520962972928068</v>
+      </c>
+      <c r="C111" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1.358024691358025</v>
+      </c>
+      <c r="E111" t="n">
+        <v>2.445790460771442</v>
+      </c>
+      <c r="F111" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -1807,15 +2778,18 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>5</v>
+        <v>4.74996074526122</v>
       </c>
       <c r="C112" t="n">
-        <v>3</v>
+        <v>3.17</v>
       </c>
       <c r="D112" t="n">
-        <v>3</v>
+        <v>3.375</v>
       </c>
       <c r="E112" t="n">
+        <v>2.859866768739055</v>
+      </c>
+      <c r="F112" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1826,15 +2800,18 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>16</v>
+        <v>15.86707009327846</v>
       </c>
       <c r="C113" t="n">
-        <v>16</v>
+        <v>15.76</v>
       </c>
       <c r="D113" t="n">
-        <v>11</v>
+        <v>10.6</v>
       </c>
       <c r="E113" t="n">
+        <v>13.32179806694158</v>
+      </c>
+      <c r="F113" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1845,15 +2822,18 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>5</v>
+        <v>5.476783751318685</v>
       </c>
       <c r="C114" t="n">
-        <v>4</v>
+        <v>4.08</v>
       </c>
       <c r="D114" t="n">
-        <v>4</v>
+        <v>3.909090909090909</v>
       </c>
       <c r="E114" t="n">
+        <v>3.904971640333383</v>
+      </c>
+      <c r="F114" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1863,6 +2843,21 @@
           <t>Puerto Rico</t>
         </is>
       </c>
+      <c r="B115" t="n">
+        <v>3.147397168178216</v>
+      </c>
+      <c r="C115" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="D115" t="n">
+        <v>4</v>
+      </c>
+      <c r="E115" t="n">
+        <v>5.816484648185696</v>
+      </c>
+      <c r="F115" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -1871,16 +2866,19 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>3</v>
+        <v>3.401238773079328</v>
       </c>
       <c r="C116" t="n">
-        <v>4</v>
+        <v>3.65</v>
       </c>
       <c r="D116" t="n">
         <v>4</v>
       </c>
       <c r="E116" t="n">
-        <v>0</v>
+        <v>0.3988345808364357</v>
+      </c>
+      <c r="F116" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="117">
@@ -1889,6 +2887,21 @@
           <t>ROC</t>
         </is>
       </c>
+      <c r="B117" t="n">
+        <v>52.69252275703983</v>
+      </c>
+      <c r="C117" t="n">
+        <v>73.75</v>
+      </c>
+      <c r="D117" t="n">
+        <v>71</v>
+      </c>
+      <c r="E117" t="n">
+        <v>72.3473536380537</v>
+      </c>
+      <c r="F117" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -1896,6 +2909,21 @@
           <t>Refugee Olympic Team</t>
         </is>
       </c>
+      <c r="B118" t="n">
+        <v>2.623789281546387</v>
+      </c>
+      <c r="C118" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D118" t="n">
+        <v>4</v>
+      </c>
+      <c r="E118" t="n">
+        <v>4.201243708502555</v>
+      </c>
+      <c r="F118" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -1904,15 +2932,18 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>10</v>
+        <v>10.28115692708276</v>
       </c>
       <c r="C119" t="n">
-        <v>11</v>
+        <v>10.79</v>
       </c>
       <c r="D119" t="n">
         <v>13</v>
       </c>
       <c r="E119" t="n">
+        <v>9.729124683727171</v>
+      </c>
+      <c r="F119" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1922,6 +2953,21 @@
           <t>Russia</t>
         </is>
       </c>
+      <c r="B120" t="n">
+        <v>52.81966732025975</v>
+      </c>
+      <c r="C120" t="n">
+        <v>105.02</v>
+      </c>
+      <c r="D120" t="n">
+        <v>112</v>
+      </c>
+      <c r="E120" t="n">
+        <v>70.22617372331794</v>
+      </c>
+      <c r="F120" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -1929,6 +2975,11 @@
           <t>Russian Empire</t>
         </is>
       </c>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr"/>
+      <c r="F121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -1936,6 +2987,21 @@
           <t>Saint Lucia</t>
         </is>
       </c>
+      <c r="B122" t="n">
+        <v>3.037425160455797</v>
+      </c>
+      <c r="C122" t="n">
+        <v>1.526666666666667</v>
+      </c>
+      <c r="D122" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0.4257598284327404</v>
+      </c>
+      <c r="F122" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -1943,6 +3009,11 @@
           <t>Samoa</t>
         </is>
       </c>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -1950,6 +3021,21 @@
           <t>San Marino</t>
         </is>
       </c>
+      <c r="B124" t="n">
+        <v>2.521500667446148</v>
+      </c>
+      <c r="C124" t="n">
+        <v>1.726666666666667</v>
+      </c>
+      <c r="D124" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E124" t="n">
+        <v>1.440905125823135</v>
+      </c>
+      <c r="F124" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -1957,6 +3043,21 @@
           <t>Saudi Arabia</t>
         </is>
       </c>
+      <c r="B125" t="n">
+        <v>2.536304762906489</v>
+      </c>
+      <c r="C125" t="n">
+        <v>1.816666666666667</v>
+      </c>
+      <c r="D125" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E125" t="n">
+        <v>2.384156265908703</v>
+      </c>
+      <c r="F125" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -1964,6 +3065,11 @@
           <t>Senegal</t>
         </is>
       </c>
+      <c r="B126" t="inlineStr"/>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -1972,16 +3078,19 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>7</v>
+        <v>6.761161930274994</v>
       </c>
       <c r="C127" t="n">
+        <v>5.36</v>
+      </c>
+      <c r="D127" t="n">
+        <v>4.176470588235294</v>
+      </c>
+      <c r="E127" t="n">
+        <v>5.876692233963919</v>
+      </c>
+      <c r="F127" t="n">
         <v>5</v>
-      </c>
-      <c r="D127" t="n">
-        <v>4</v>
-      </c>
-      <c r="E127" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="128">
@@ -1990,6 +3099,31 @@
           <t>Serbia and Montenegro</t>
         </is>
       </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -1997,6 +3131,21 @@
           <t>Singapore</t>
         </is>
       </c>
+      <c r="B129" t="n">
+        <v>2.808379466545567</v>
+      </c>
+      <c r="C129" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="D129" t="n">
+        <v>2.285714285714286</v>
+      </c>
+      <c r="E129" t="n">
+        <v>3.675498886488101</v>
+      </c>
+      <c r="F129" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2005,16 +3154,19 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>3</v>
+        <v>3.429171576632086</v>
       </c>
       <c r="C130" t="n">
-        <v>3</v>
+        <v>3.15</v>
       </c>
       <c r="D130" t="n">
-        <v>3</v>
+        <v>3.375</v>
       </c>
       <c r="E130" t="n">
-        <v>1</v>
+        <v>0.8888479268116942</v>
+      </c>
+      <c r="F130" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="131">
@@ -2024,15 +3176,18 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>5</v>
+        <v>4.918483579829271</v>
       </c>
       <c r="C131" t="n">
-        <v>4</v>
+        <v>3.71</v>
       </c>
       <c r="D131" t="n">
         <v>1</v>
       </c>
       <c r="E131" t="n">
+        <v>3.390238169524491</v>
+      </c>
+      <c r="F131" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2043,16 +3198,19 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>7</v>
+        <v>7.169053014461625</v>
       </c>
       <c r="C132" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="D132" t="n">
+        <v>4.176470588235294</v>
+      </c>
+      <c r="E132" t="n">
+        <v>6.432826777150311</v>
+      </c>
+      <c r="F132" t="n">
         <v>5</v>
-      </c>
-      <c r="D132" t="n">
-        <v>4</v>
-      </c>
-      <c r="E132" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="133">
@@ -2062,16 +3220,19 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>36</v>
+        <v>36.42756734187029</v>
       </c>
       <c r="C133" t="n">
-        <v>30</v>
+        <v>30.39</v>
       </c>
       <c r="D133" t="n">
         <v>37</v>
       </c>
       <c r="E133" t="n">
-        <v>32</v>
+        <v>32.49758844423143</v>
+      </c>
+      <c r="F133" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="134">
@@ -2100,6 +3261,11 @@
           <t>ABSENT</t>
         </is>
       </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2108,16 +3274,19 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>27</v>
+        <v>27.05991671630196</v>
       </c>
       <c r="C135" t="n">
-        <v>26</v>
+        <v>26.14</v>
       </c>
       <c r="D135" t="n">
         <v>37</v>
       </c>
       <c r="E135" t="n">
-        <v>22</v>
+        <v>21.69704929882647</v>
+      </c>
+      <c r="F135" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="136">
@@ -2126,6 +3295,11 @@
           <t>Sri Lanka</t>
         </is>
       </c>
+      <c r="B136" t="inlineStr"/>
+      <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="inlineStr"/>
+      <c r="F136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2133,6 +3307,11 @@
           <t>Sudan</t>
         </is>
       </c>
+      <c r="B137" t="inlineStr"/>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
+      <c r="E137" t="inlineStr"/>
+      <c r="F137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2140,6 +3319,11 @@
           <t>Suriname</t>
         </is>
       </c>
+      <c r="B138" t="inlineStr"/>
+      <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="inlineStr"/>
+      <c r="F138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2148,15 +3332,18 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>10</v>
+        <v>9.748041696508437</v>
       </c>
       <c r="C139" t="n">
-        <v>11</v>
+        <v>11.09</v>
       </c>
       <c r="D139" t="n">
         <v>14</v>
       </c>
       <c r="E139" t="n">
+        <v>11.27130699791874</v>
+      </c>
+      <c r="F139" t="n">
         <v>11</v>
       </c>
     </row>
@@ -2167,16 +3354,19 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>11</v>
+        <v>10.51575316453427</v>
       </c>
       <c r="C140" t="n">
-        <v>10</v>
+        <v>9.66</v>
       </c>
       <c r="D140" t="n">
-        <v>10</v>
+        <v>9.76923076923077</v>
       </c>
       <c r="E140" t="n">
-        <v>10</v>
+        <v>9.571151865446634</v>
+      </c>
+      <c r="F140" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="141">
@@ -2185,6 +3375,21 @@
           <t>Syria</t>
         </is>
       </c>
+      <c r="B141" t="n">
+        <v>2.459499148638677</v>
+      </c>
+      <c r="C141" t="n">
+        <v>1.677047619047619</v>
+      </c>
+      <c r="D141" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E141" t="n">
+        <v>1.019115754261196</v>
+      </c>
+      <c r="F141" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2192,6 +3397,11 @@
           <t>Taiwan</t>
         </is>
       </c>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
+      <c r="E142" t="inlineStr"/>
+      <c r="F142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2199,6 +3409,21 @@
           <t>Tajikistan</t>
         </is>
       </c>
+      <c r="B143" t="n">
+        <v>3.055525526269427</v>
+      </c>
+      <c r="C143" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="D143" t="n">
+        <v>2</v>
+      </c>
+      <c r="E143" t="n">
+        <v>1.553460195191556</v>
+      </c>
+      <c r="F143" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2206,6 +3431,11 @@
           <t>Tanzania</t>
         </is>
       </c>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2214,16 +3444,19 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>5</v>
+        <v>5.13172499426959</v>
       </c>
       <c r="C145" t="n">
-        <v>5</v>
+        <v>5.32</v>
       </c>
       <c r="D145" t="n">
         <v>1</v>
       </c>
       <c r="E145" t="n">
-        <v>5</v>
+        <v>4.741280265289236</v>
+      </c>
+      <c r="F145" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="146">
@@ -2232,6 +3465,11 @@
           <t>Togo</t>
         </is>
       </c>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -2239,6 +3477,11 @@
           <t>Tonga</t>
         </is>
       </c>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
+      <c r="E147" t="inlineStr"/>
+      <c r="F147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2246,6 +3489,21 @@
           <t>Trinidad and Tobago</t>
         </is>
       </c>
+      <c r="B148" t="n">
+        <v>3.75591806295914</v>
+      </c>
+      <c r="C148" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="D148" t="n">
+        <v>2.285714285714286</v>
+      </c>
+      <c r="E148" t="n">
+        <v>4.793364594482297</v>
+      </c>
+      <c r="F148" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2254,16 +3512,19 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>4</v>
+        <v>4.092393248310856</v>
       </c>
       <c r="C149" t="n">
-        <v>4</v>
+        <v>3.79</v>
       </c>
       <c r="D149" t="n">
-        <v>4</v>
+        <v>3.909090909090909</v>
       </c>
       <c r="E149" t="n">
-        <v>2</v>
+        <v>2.394785163495753</v>
+      </c>
+      <c r="F149" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="150">
@@ -2273,15 +3534,18 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>9</v>
+        <v>8.510520219599208</v>
       </c>
       <c r="C150" t="n">
-        <v>9</v>
+        <v>9.02</v>
       </c>
       <c r="D150" t="n">
-        <v>10</v>
+        <v>9.76923076923077</v>
       </c>
       <c r="E150" t="n">
+        <v>8.340006499268188</v>
+      </c>
+      <c r="F150" t="n">
         <v>8</v>
       </c>
     </row>
@@ -2291,6 +3555,21 @@
           <t>Turkmenistan</t>
         </is>
       </c>
+      <c r="B151" t="n">
+        <v>2.467589962358041</v>
+      </c>
+      <c r="C151" t="n">
+        <v>1.707047619047619</v>
+      </c>
+      <c r="D151" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0.9728256071262642</v>
+      </c>
+      <c r="F151" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -2298,6 +3577,21 @@
           <t>Uganda</t>
         </is>
       </c>
+      <c r="B152" t="n">
+        <v>2.854661057057875</v>
+      </c>
+      <c r="C152" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="D152" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E152" t="n">
+        <v>3.921587170424478</v>
+      </c>
+      <c r="F152" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2306,16 +3600,19 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>15</v>
+        <v>14.72251198773009</v>
       </c>
       <c r="C153" t="n">
-        <v>11</v>
+        <v>10.95</v>
       </c>
       <c r="D153" t="n">
         <v>12</v>
       </c>
       <c r="E153" t="n">
-        <v>14</v>
+        <v>14.05247179015959</v>
+      </c>
+      <c r="F153" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="154">
@@ -2324,6 +3621,31 @@
           <t>Unified Team</t>
         </is>
       </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -2331,6 +3653,21 @@
           <t>United Arab Emirates</t>
         </is>
       </c>
+      <c r="B155" t="n">
+        <v>2.581928669905771</v>
+      </c>
+      <c r="C155" t="n">
+        <v>1.768809523809524</v>
+      </c>
+      <c r="D155" t="n">
+        <v>1.25609756097561</v>
+      </c>
+      <c r="E155" t="n">
+        <v>0.2337790593895708</v>
+      </c>
+      <c r="F155" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -2339,16 +3676,19 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>107</v>
+        <v>107.3702659849647</v>
       </c>
       <c r="C156" t="n">
-        <v>165</v>
+        <v>165.08</v>
       </c>
       <c r="D156" t="n">
         <v>195</v>
       </c>
       <c r="E156" t="n">
-        <v>125</v>
+        <v>124.8513782597464</v>
+      </c>
+      <c r="F156" t="n">
+        <v>148</v>
       </c>
     </row>
     <row r="157">
@@ -2357,6 +3697,11 @@
           <t>United Team of Germany</t>
         </is>
       </c>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" t="inlineStr"/>
+      <c r="D157" t="inlineStr"/>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -2364,6 +3709,11 @@
           <t>Uruguay</t>
         </is>
       </c>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -2372,16 +3722,19 @@
         </is>
       </c>
       <c r="B159" t="n">
+        <v>9.408801229771484</v>
+      </c>
+      <c r="C159" t="n">
+        <v>9.41</v>
+      </c>
+      <c r="D159" t="n">
+        <v>9.76923076923077</v>
+      </c>
+      <c r="E159" t="n">
+        <v>10.76434924259609</v>
+      </c>
+      <c r="F159" t="n">
         <v>9</v>
-      </c>
-      <c r="C159" t="n">
-        <v>9</v>
-      </c>
-      <c r="D159" t="n">
-        <v>10</v>
-      </c>
-      <c r="E159" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="160">
@@ -2390,6 +3743,21 @@
           <t>Venezuela</t>
         </is>
       </c>
+      <c r="B160" t="n">
+        <v>2.783517853519768</v>
+      </c>
+      <c r="C160" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="D160" t="n">
+        <v>4</v>
+      </c>
+      <c r="E160" t="n">
+        <v>7.265864874649763</v>
+      </c>
+      <c r="F160" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -2397,6 +3765,21 @@
           <t>Vietnam</t>
         </is>
       </c>
+      <c r="B161" t="n">
+        <v>2.524273223648237</v>
+      </c>
+      <c r="C161" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="D161" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E161" t="n">
+        <v>1.382096789852355</v>
+      </c>
+      <c r="F161" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -2404,6 +3787,11 @@
           <t>Virgin Islands</t>
         </is>
       </c>
+      <c r="B162" t="inlineStr"/>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
+      <c r="E162" t="inlineStr"/>
+      <c r="F162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -2431,6 +3819,11 @@
           <t>ABSENT</t>
         </is>
       </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -2458,6 +3851,11 @@
           <t>ABSENT</t>
         </is>
       </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -2465,6 +3863,21 @@
           <t>Zambia</t>
         </is>
       </c>
+      <c r="B165" t="n">
+        <v>2.609972461255062</v>
+      </c>
+      <c r="C165" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="D165" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E165" t="n">
+        <v>1.340033807610968</v>
+      </c>
+      <c r="F165" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -2472,6 +3885,11 @@
           <t>Zimbabwe</t>
         </is>
       </c>
+      <c r="B166" t="inlineStr"/>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr"/>
+      <c r="F166" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>